<commit_message>
made changes in payment script and base file also enhanced code and made changes in assert
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sthapatya\eclipse-workspace\New_Web_Automation_Script\InputData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="8160"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>UserId</t>
   </si>
@@ -58,18 +62,9 @@
     <t>Payment mode</t>
   </si>
   <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Cheque-clear</t>
-  </si>
-  <si>
     <t>Card</t>
   </si>
   <si>
-    <t>advance</t>
-  </si>
-  <si>
     <t>PMC</t>
   </si>
   <si>
@@ -85,15 +80,6 @@
     <t>User@1234</t>
   </si>
   <si>
-    <t>KM</t>
-  </si>
-  <si>
-    <t>Cheque-Fail</t>
-  </si>
-  <si>
-    <t>node5</t>
-  </si>
-  <si>
     <t>node1</t>
   </si>
   <si>
@@ -106,34 +92,28 @@
     <t>node4</t>
   </si>
   <si>
-    <t>node6</t>
-  </si>
-  <si>
-    <t>node7</t>
-  </si>
-  <si>
-    <t>node8</t>
-  </si>
-  <si>
-    <t>node9</t>
-  </si>
-  <si>
-    <t>http://testpanvelmc.ptaxcollection.com:8080/Pages/Login.aspx</t>
-  </si>
-  <si>
-    <t>Testing properties for payment Baramati</t>
-  </si>
-  <si>
-    <t>11-1</t>
-  </si>
-  <si>
-    <t>22-1</t>
-  </si>
-  <si>
-    <t>KL</t>
-  </si>
-  <si>
-    <t>50-1</t>
+    <t>Cheque-bounce</t>
+  </si>
+  <si>
+    <t>Cheque-Clear</t>
+  </si>
+  <si>
+    <t>Cash+advance</t>
+  </si>
+  <si>
+    <t>BMC</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>99</t>
   </si>
 </sst>
 </file>
@@ -191,7 +171,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -224,26 +204,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
@@ -259,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -292,25 +252,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -597,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,14 +583,14 @@
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
-        <v>123</v>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5">
         <v>6</v>
@@ -662,10 +607,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5">
         <v>1</v>
@@ -681,13 +626,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -698,11 +643,11 @@
       <c r="E7" s="8"/>
     </row>
     <row r="8" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
       <c r="D8" s="9"/>
       <c r="E8" s="8"/>
     </row>
@@ -723,202 +668,80 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B10" s="11">
-        <v>10</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>34</v>
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>26</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="14">
-        <v>14</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>34</v>
+        <v>25</v>
+      </c>
+      <c r="B11" s="11">
+        <v>4</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="11">
+        <v>4</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="11">
+        <v>4</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="1">
-        <v>20</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="11">
-        <v>10</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="11">
-        <v>10</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="14">
-        <v>14</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="1">
-        <v>20</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="11">
-        <v>10</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B20" s="1">
-        <v>20</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2" display="User@1234"/>
-    <hyperlink ref="C2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add test output files
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -544,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated pcmc code of payments and reports
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sthapatya\eclipse-workspace\New_Web_Automation_Script\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\Web_Automation_Script\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>UserId</t>
   </si>
@@ -104,16 +104,19 @@
     <t>BMC</t>
   </si>
   <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>20</t>
   </si>
   <si>
-    <t>99</t>
+    <t>131</t>
+  </si>
+  <si>
+    <t>TRG</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
   </si>
 </sst>
 </file>
@@ -545,7 +548,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,13 +584,13 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="B2" s="7">
+        <v>123</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>25</v>
@@ -668,13 +671,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B10" s="11">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>24</v>
@@ -685,13 +688,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B11" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>22</v>
@@ -708,7 +711,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>23</v>
@@ -719,13 +722,13 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B13" s="11">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
integrated db and made changes in payment script
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\eclipse-workspace\Web_Automation_Script\InputData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sthapatya\eclipse-workspace\New_Web_Automation_Script\InputData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
   <si>
     <t>UserId</t>
   </si>
@@ -101,19 +101,25 @@
     <t>Cash+advance</t>
   </si>
   <si>
-    <t>13-7</t>
-  </si>
-  <si>
-    <t>BMC</t>
-  </si>
-  <si>
-    <t>76-6</t>
-  </si>
-  <si>
-    <t>68-2</t>
-  </si>
-  <si>
-    <t>840-5</t>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>http://testpanvelmc.ptaxcollection.com:8080/Pages/Login.aspx</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>1-101</t>
+  </si>
+  <si>
+    <t>1-14</t>
+  </si>
+  <si>
+    <t>1-26</t>
+  </si>
+  <si>
+    <t>1-28</t>
   </si>
 </sst>
 </file>
@@ -545,7 +551,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,17 +589,17 @@
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>7</v>
+      <c r="B2" s="7">
+        <v>123</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F2" s="5">
         <v>2024</v>
@@ -668,13 +674,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>24</v>
@@ -685,13 +691,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>22</v>
@@ -702,13 +708,13 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="11">
         <v>1</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>23</v>
@@ -719,13 +725,13 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B13" s="11">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
done changes in payment and removed excel from logic
</commit_message>
<xml_diff>
--- a/InputData/CMS Data.xlsx
+++ b/InputData/CMS Data.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sthapatya\eclipse-workspace\New_Web_Automation_Script\InputData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17040" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24435" windowHeight="6615"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
   <si>
     <t>UserId</t>
   </si>
@@ -102,9 +98,6 @@
   </si>
   <si>
     <t>KM</t>
-  </si>
-  <si>
-    <t>http://testpanvelmc.ptaxcollection.com:8080/Pages/Login.aspx</t>
   </si>
   <si>
     <t>KH</t>
@@ -551,7 +544,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -589,11 +582,11 @@
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="7">
-        <v>123</v>
+      <c r="B2" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>25</v>
@@ -674,13 +667,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="11">
         <v>1</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>24</v>
@@ -691,13 +684,13 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="11">
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>22</v>
@@ -708,13 +701,13 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="11">
         <v>1</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>23</v>
@@ -725,13 +718,13 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="11">
         <v>1</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>12</v>

</xml_diff>